<commit_message>
Spreadsheet with global measurements
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/bsort_alu_verify/bsort_alu_verify_measurements.xlsx
+++ b/verilog/hardware/processor/source/bsort_alu_verify/bsort_alu_verify_measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/bsort_alu_verify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8059583-3652-674A-B149-DB39DBECCB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013DA161-CC05-FD4E-BEB7-6BDC175708F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
+    <workbookView xWindow="3880" yWindow="2200" windowWidth="16700" windowHeight="17440" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -508,6 +508,9 @@
       <c r="C3" s="2">
         <v>4.1321500000000002E-3</v>
       </c>
+      <c r="D3" s="4">
+        <v>10.47</v>
+      </c>
       <c r="E3" s="5">
         <v>3238</v>
       </c>
@@ -519,6 +522,9 @@
       <c r="C4" s="4">
         <v>7.58203E-3</v>
       </c>
+      <c r="D4" s="4">
+        <v>20.95</v>
+      </c>
       <c r="E4" s="5">
         <v>3238</v>
       </c>
@@ -530,6 +536,9 @@
       <c r="C5" s="4">
         <v>4.2287499999999999E-3</v>
       </c>
+      <c r="D5" s="4">
+        <v>10.465</v>
+      </c>
       <c r="E5" s="5">
         <v>3270</v>
       </c>
@@ -541,6 +550,9 @@
       <c r="C6" s="4">
         <v>4.00118E-3</v>
       </c>
+      <c r="D6" s="4">
+        <v>10.49</v>
+      </c>
       <c r="E6" s="5">
         <v>3270</v>
       </c>
@@ -552,6 +564,9 @@
       <c r="C7" s="4">
         <v>4.0526E-3</v>
       </c>
+      <c r="D7" s="4">
+        <v>10.43</v>
+      </c>
       <c r="E7" s="5">
         <v>3247</v>
       </c>
@@ -563,6 +578,9 @@
       <c r="C8" s="4">
         <v>4.0426100000000003E-3</v>
       </c>
+      <c r="D8" s="4">
+        <v>10.35</v>
+      </c>
       <c r="E8" s="5">
         <v>3222</v>
       </c>
@@ -574,6 +592,9 @@
       <c r="C9" s="4">
         <v>4.4236600000000003E-3</v>
       </c>
+      <c r="D9" s="4">
+        <v>10.46</v>
+      </c>
       <c r="E9" s="5">
         <v>3180</v>
       </c>
@@ -593,6 +614,9 @@
       <c r="C11" s="4">
         <v>3.87594E-3</v>
       </c>
+      <c r="D11" s="4">
+        <v>10.46</v>
+      </c>
       <c r="E11" s="5">
         <v>3216</v>
       </c>
@@ -604,6 +628,9 @@
       <c r="C12" s="4">
         <v>4.1336799999999998E-3</v>
       </c>
+      <c r="D12" s="4">
+        <v>10.465</v>
+      </c>
       <c r="E12" s="5">
         <v>3238</v>
       </c>
@@ -623,6 +650,9 @@
       <c r="C14" s="4">
         <v>5.7999599999999998E-3</v>
       </c>
+      <c r="D14" s="4">
+        <v>6.96</v>
+      </c>
       <c r="E14" s="5">
         <v>3246</v>
       </c>
@@ -633,6 +663,9 @@
       </c>
       <c r="C15" s="4">
         <v>2.5024000000000001E-3</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="E15" s="5">
         <v>3238</v>

</xml_diff>

<commit_message>
add CPI and nJ/op
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/bsort_alu_verify/bsort_alu_verify_measurements.xlsx
+++ b/verilog/hardware/processor/source/bsort_alu_verify/bsort_alu_verify_measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/bsort_alu_verify/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\f-of-e-tools\verilog\hardware\processor\source\bsort_alu_verify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013DA161-CC05-FD4E-BEB7-6BDC175708F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF19294E-C3D7-4B1F-BA45-C88DF834F467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="2200" windowWidth="16700" windowHeight="17440" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="27000" windowHeight="14235" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>bsort_alu_verify MEASUREMENTS</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>PLL_12.5MHz</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>nJ per instruction</t>
   </si>
 </sst>
 </file>
@@ -160,7 +166,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,21 +478,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5514D7BD-1B29-5548-99C9-D3A14905CC46}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.83203125" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="4"/>
-    <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="62.875" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="4"/>
+    <col min="5" max="5" width="10.875" style="5"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +507,14 @@
       <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -514,8 +527,16 @@
       <c r="E3" s="5">
         <v>3238</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f>6000000/(D3*192000)</f>
+        <v>2.9847182425978982</v>
+      </c>
+      <c r="G3">
+        <f>C3/D3/192000*1000000000</f>
+        <v>2.0555505810251513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -528,8 +549,16 @@
       <c r="E4" s="5">
         <v>3238</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>12000000/(D4*192000)</f>
+        <v>2.9832935560859188</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G19" si="0">C4/D4/192000*1000000000</f>
+        <v>1.88495177008751</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -542,8 +571,16 @@
       <c r="E5" s="5">
         <v>3270</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" ref="F4:F19" si="1">6000000/(D5*192000)</f>
+        <v>2.9861442904921165</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.1046096114030894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -556,8 +593,16 @@
       <c r="E6" s="5">
         <v>3270</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2.979027645376549</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.9866043056879568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -570,8 +615,16 @@
       <c r="E7" s="5">
         <v>3247</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>2.9961649089165867</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>2.023709651645893</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -584,8 +637,16 @@
       <c r="E8" s="5">
         <v>3222</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>3.0193236714975846</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2.0343246779388084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -598,16 +659,32 @@
       <c r="E9" s="5">
         <v>3180</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>2.987571701720841</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.2026669056724026</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="5">
         <v>3238</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -620,8 +697,16 @@
       <c r="E11" s="5">
         <v>3216</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>2.987571701720841</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1.929941443594646</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -634,16 +719,32 @@
       <c r="E12" s="5">
         <v>3238</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>2.9861442904921165</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.0572941551202417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="5">
         <v>3238</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -656,8 +757,16 @@
       <c r="E14" s="5">
         <v>3246</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f>4000000/(D14*192000)</f>
+        <v>2.9932950191570882</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>4.3402478448275854</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -670,37 +779,77 @@
       <c r="E15" s="5">
         <v>3238</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f>10000/(D15*192000)</f>
+        <v>2.9932950191570882</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>749.04214559386992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="4">
         <v>1.1715339999999999E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="5">
         <v>3195</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="5">
         <v>3205</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="5">
         <v>3205</v>
+      </c>
+      <c r="F19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>